<commit_message>
Fix typo (STRIP8 instead of STRIP08) in Excel tables
</commit_message>
<xml_diff>
--- a/data/default_biases_cryo.xlsx
+++ b/data/default_biases_cryo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="5960"/>
+    <workbookView activeTab="1" windowWidth="14400" windowHeight="5960"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55" count="55">
   <si>
-    <t>PAR</t>
-  </si>
-  <si>
     <t>STRIP02</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>STRIP07</t>
+  </si>
+  <si>
+    <t>STRIP08</t>
   </si>
   <si>
     <t>STRIP09</t>
@@ -289,8 +289,8 @@
   </sheetPr>
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -299,25 +299,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67">
-      <c r="A1" t="s">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>PAR</t>
+        </is>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>STRIP08</t>
-        </is>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -6284,8 +6284,8 @@
   </sheetPr>
   <dimension ref="A1:AMK1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A8" workbookViewId="0" tabSelected="1">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6360,7 +6360,7 @@
         </is>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1025" ht="20.25">
@@ -6574,10 +6574,8 @@
           <t>Y0</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>STRIP8</t>
-        </is>
+      <c r="B26" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:1025" ht="20.25">
@@ -6607,7 +6605,7 @@
         </is>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:1025" ht="20.25">
@@ -6702,7 +6700,7 @@
         </is>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:1025" ht="20.25">
@@ -6757,7 +6755,7 @@
         </is>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:1025" ht="20.25">

</xml_diff>

<commit_message>
Set detector offset and gain to zero for cryo biases
</commit_message>
<xml_diff>
--- a/data/default_biases_cryo.xlsx
+++ b/data/default_biases_cryo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11472" windowHeight="9216"/>
+    <workbookView windowWidth="23040" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" r:id="rId1"/>
@@ -1503,8 +1503,8 @@
   <sheetPr/>
   <dimension ref="A1:BO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -8217,202 +8217,202 @@
         <v>99</v>
       </c>
       <c r="B34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO34" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" ht="13.2" spans="1:67">
@@ -8420,202 +8420,202 @@
         <v>100</v>
       </c>
       <c r="B35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO35" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="13.2" spans="1:67">
@@ -8623,202 +8623,202 @@
         <v>101</v>
       </c>
       <c r="B36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO36" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" ht="13.2" spans="1:67">
@@ -8826,202 +8826,202 @@
         <v>102</v>
       </c>
       <c r="B37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO37" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="13.2" spans="1:67">
@@ -9029,202 +9029,202 @@
         <v>103</v>
       </c>
       <c r="B38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO38" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" ht="13.2" spans="1:67">
@@ -9232,202 +9232,202 @@
         <v>104</v>
       </c>
       <c r="B39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO39" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" ht="13.2" spans="1:67">
@@ -9435,202 +9435,202 @@
         <v>105</v>
       </c>
       <c r="B40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO40" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" ht="13.2" spans="1:67">
@@ -9638,202 +9638,202 @@
         <v>106</v>
       </c>
       <c r="B41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="P41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="R41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="S41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="T41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="V41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="X41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Y41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AB41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AD41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AE41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AF41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AG41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AH41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AI41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AJ41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AK41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AL41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AN41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AO41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AP41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AQ41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AR41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AS41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AT41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AU41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AV41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AW41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AX41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AY41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AZ41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BA41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BB41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BC41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BD41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BE41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BF41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BG41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BH41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BI41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BJ41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BK41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BL41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BM41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BN41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="BO41" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set cryo pretuning and default biases
</commit_message>
<xml_diff>
--- a/data/default_biases_cryo.xlsx
+++ b/data/default_biases_cryo.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\zec\striptease\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F2EE7D-D14B-4B91-95E6-C1E84250819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Biases" sheetId="1" r:id="rId1"/>
     <sheet name="Modules" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Biases"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Modules"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -539,14 +545,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -566,159 +566,8 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,194 +580,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -926,318 +589,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1495,25 +872,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AC18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.8888888888889" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.13888888888889" style="3"/>
+    <col min="1" max="1" width="16.85546875" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.2" spans="1:67">
+    <row r="1" spans="1:67">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1096,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" ht="13.2" spans="1:67">
+    <row r="2" spans="1:67">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1919,7 +1299,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" ht="13.2" spans="1:67">
+    <row r="3" spans="1:67">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2122,7 +1502,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" ht="13.2" spans="1:67">
+    <row r="4" spans="1:67">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -2325,7 +1705,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" ht="13.2" spans="1:67">
+    <row r="5" spans="1:67">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -2528,7 +1908,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="6" ht="13.2" spans="1:67">
+    <row r="6" spans="1:67">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -2731,7 +2111,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" ht="13.2" spans="1:67">
+    <row r="7" spans="1:67">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -2934,7 +2314,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" ht="13.2" spans="1:67">
+    <row r="8" spans="1:67">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -3137,7 +2517,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" ht="13.2" spans="1:67">
+    <row r="9" spans="1:67">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -3340,7 +2720,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="10" ht="13.2" spans="1:67">
+    <row r="10" spans="1:67">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -3543,7 +2923,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" ht="13.2" spans="1:67">
+    <row r="11" spans="1:67">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -3746,7 +3126,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" ht="13.2" spans="1:67">
+    <row r="12" spans="1:67">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -3949,7 +3329,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="13" ht="13.2" spans="1:67">
+    <row r="13" spans="1:67">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -4152,7 +3532,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" ht="13.2" spans="1:67">
+    <row r="14" spans="1:67">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -4355,7 +3735,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" ht="13.2" spans="1:67">
+    <row r="15" spans="1:67">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -4558,7 +3938,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" ht="13.2" spans="1:67">
+    <row r="16" spans="1:67">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -4761,7 +4141,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="17" ht="13.2" spans="1:67">
+    <row r="17" spans="1:67">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -4964,7 +4344,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="18" ht="13.2" spans="1:67">
+    <row r="18" spans="1:67">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -5167,7 +4547,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="19" ht="13.2" spans="1:67">
+    <row r="19" spans="1:67">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -5370,7 +4750,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="20" ht="13.2" spans="1:67">
+    <row r="20" spans="1:67">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -5573,7 +4953,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" ht="13.2" spans="1:67">
+    <row r="21" spans="1:67">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -5776,7 +5156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" ht="13.2" spans="1:67">
+    <row r="22" spans="1:67">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -5979,7 +5359,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" ht="13.2" spans="1:67">
+    <row r="23" spans="1:67">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -6182,7 +5562,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" ht="13.2" spans="1:67">
+    <row r="24" spans="1:67">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -6385,7 +5765,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="25" ht="13.2" spans="1:67">
+    <row r="25" spans="1:67">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -6588,7 +5968,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="26" ht="13.2" spans="1:67">
+    <row r="26" spans="1:67">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -6791,7 +6171,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="27" ht="13.2" spans="1:67">
+    <row r="27" spans="1:67">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -6994,7 +6374,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="28" ht="13.2" spans="1:67">
+    <row r="28" spans="1:67">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -7197,7 +6577,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="29" ht="13.2" spans="1:67">
+    <row r="29" spans="1:67">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -7400,7 +6780,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" ht="13.2" spans="1:67">
+    <row r="30" spans="1:67">
       <c r="A30" s="4" t="s">
         <v>95</v>
       </c>
@@ -7603,7 +6983,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" ht="13.2" spans="1:67">
+    <row r="31" spans="1:67">
       <c r="A31" s="4" t="s">
         <v>96</v>
       </c>
@@ -7806,7 +7186,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" ht="13.2" spans="1:67">
+    <row r="32" spans="1:67">
       <c r="A32" s="4" t="s">
         <v>97</v>
       </c>
@@ -8009,7 +7389,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" ht="13.2" spans="1:67">
+    <row r="33" spans="1:67">
       <c r="A33" s="4" t="s">
         <v>98</v>
       </c>
@@ -8212,7 +7592,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" ht="13.2" spans="1:67">
+    <row r="34" spans="1:67">
       <c r="A34" s="4" t="s">
         <v>99</v>
       </c>
@@ -8247,7 +7627,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="4">
-        <v>0</v>
+        <v>2170</v>
       </c>
       <c r="M34" s="4">
         <v>0</v>
@@ -8301,7 +7681,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="4">
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="AE34" s="4">
         <v>0</v>
@@ -8322,7 +7702,7 @@
         <v>0</v>
       </c>
       <c r="AK34" s="4">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="AL34" s="4">
         <v>0</v>
@@ -8382,7 +7762,7 @@
         <v>0</v>
       </c>
       <c r="BE34" s="4">
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="BF34" s="4">
         <v>0</v>
@@ -8415,7 +7795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" ht="13.2" spans="1:67">
+    <row r="35" spans="1:67">
       <c r="A35" s="4" t="s">
         <v>100</v>
       </c>
@@ -8450,7 +7830,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="4">
-        <v>0</v>
+        <v>2170</v>
       </c>
       <c r="M35" s="4">
         <v>0</v>
@@ -8504,7 +7884,7 @@
         <v>0</v>
       </c>
       <c r="AD35" s="4">
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="AE35" s="4">
         <v>0</v>
@@ -8525,7 +7905,7 @@
         <v>0</v>
       </c>
       <c r="AK35" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="AL35" s="4">
         <v>0</v>
@@ -8585,7 +7965,7 @@
         <v>0</v>
       </c>
       <c r="BE35" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="BF35" s="4">
         <v>0</v>
@@ -8618,7 +7998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" ht="13.2" spans="1:67">
+    <row r="36" spans="1:67">
       <c r="A36" s="4" t="s">
         <v>101</v>
       </c>
@@ -8653,7 +8033,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="4">
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="M36" s="4">
         <v>0</v>
@@ -8707,7 +8087,7 @@
         <v>0</v>
       </c>
       <c r="AD36" s="4">
-        <v>0</v>
+        <v>2250</v>
       </c>
       <c r="AE36" s="4">
         <v>0</v>
@@ -8728,7 +8108,7 @@
         <v>0</v>
       </c>
       <c r="AK36" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="AL36" s="4">
         <v>0</v>
@@ -8788,7 +8168,7 @@
         <v>0</v>
       </c>
       <c r="BE36" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="BF36" s="4">
         <v>0</v>
@@ -8821,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" ht="13.2" spans="1:67">
+    <row r="37" spans="1:67">
       <c r="A37" s="4" t="s">
         <v>102</v>
       </c>
@@ -8856,7 +8236,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="4">
-        <v>0</v>
+        <v>2260</v>
       </c>
       <c r="M37" s="4">
         <v>0</v>
@@ -8910,7 +8290,7 @@
         <v>0</v>
       </c>
       <c r="AD37" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="AE37" s="4">
         <v>0</v>
@@ -8931,7 +8311,7 @@
         <v>0</v>
       </c>
       <c r="AK37" s="4">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="AL37" s="4">
         <v>0</v>
@@ -8991,7 +8371,7 @@
         <v>0</v>
       </c>
       <c r="BE37" s="4">
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="BF37" s="4">
         <v>0</v>
@@ -9024,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" ht="13.2" spans="1:67">
+    <row r="38" spans="1:67">
       <c r="A38" s="4" t="s">
         <v>103</v>
       </c>
@@ -9227,7 +8607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" ht="13.2" spans="1:67">
+    <row r="39" spans="1:67">
       <c r="A39" s="4" t="s">
         <v>104</v>
       </c>
@@ -9430,7 +8810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" ht="13.2" spans="1:67">
+    <row r="40" spans="1:67">
       <c r="A40" s="4" t="s">
         <v>105</v>
       </c>
@@ -9633,7 +9013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" ht="13.2" spans="1:67">
+    <row r="41" spans="1:67">
       <c r="A41" s="4" t="s">
         <v>106</v>
       </c>
@@ -9837,28 +9217,26 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.83333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1111111111111" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.5462962962963" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="9.13888888888889" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -9872,7 +9250,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" ht="13.2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -9880,7 +9258,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" ht="13.2" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -9888,7 +9266,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" ht="13.2" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -9896,7 +9274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="13.2" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -9904,7 +9282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" ht="13.2" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -9912,7 +9290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" ht="13.2" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -9920,7 +9298,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" ht="13.2" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -9928,7 +9306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" ht="13.2" spans="1:3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -9939,7 +9317,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" ht="13.2" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -9947,7 +9325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" ht="13.2" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -9955,7 +9333,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" ht="13.2" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -9963,7 +9341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" ht="13.2" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -9971,7 +9349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" ht="13.2" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -9979,7 +9357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" ht="13.2" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -9987,7 +9365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" ht="13.2" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -9995,7 +9373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" ht="13.2" spans="1:3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -10006,7 +9384,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" ht="13.2" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -10014,7 +9392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" ht="13.2" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -10022,7 +9400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" ht="13.2" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -10030,7 +9408,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" ht="13.2" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -10038,7 +9416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" ht="13.2" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -10046,7 +9424,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" ht="13.2" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -10054,7 +9432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" ht="13.2" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -10062,7 +9440,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" ht="13.2" spans="1:3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -10073,7 +9451,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" ht="13.2" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -10081,7 +9459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" ht="13.2" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -10089,7 +9467,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" ht="13.2" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -10097,7 +9475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" ht="13.2" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -10105,7 +9483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" ht="13.2" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -10113,7 +9491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" ht="13.2" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -10121,7 +9499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" ht="13.2" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -10129,7 +9507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" ht="13.2" spans="1:3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -10140,7 +9518,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" ht="13.2" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -10148,7 +9526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" ht="13.2" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -10156,7 +9534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" ht="13.2" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -10164,7 +9542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" ht="13.2" spans="1:2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -10172,7 +9550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" ht="13.2" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -10180,7 +9558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" ht="13.2" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -10188,7 +9566,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" ht="13.2" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -10196,7 +9574,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" ht="13.2" spans="1:3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -10207,7 +9585,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" ht="13.2" spans="1:2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -10215,7 +9593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" ht="13.2" spans="1:2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -10223,7 +9601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" ht="13.2" spans="1:2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>157</v>
       </c>
@@ -10231,7 +9609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" ht="13.2" spans="1:2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -10239,7 +9617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" ht="13.2" spans="1:2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>159</v>
       </c>
@@ -10247,7 +9625,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" ht="13.2" spans="1:2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -10255,7 +9633,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" ht="13.2" spans="1:2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>161</v>
       </c>
@@ -10263,7 +9641,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" ht="13.2" spans="1:3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>162</v>
       </c>
@@ -10274,7 +9652,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="50" ht="13.2" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>164</v>
       </c>
@@ -10282,7 +9660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" ht="13.2" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>165</v>
       </c>
@@ -10290,7 +9668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" ht="13.2" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>166</v>
       </c>
@@ -10298,7 +9676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" ht="13.2" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -10306,7 +9684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" ht="13.2" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>168</v>
       </c>
@@ -10314,7 +9692,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" ht="13.2" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -10322,7 +9700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" ht="13.2" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>170</v>
       </c>
@@ -10331,8 +9709,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="1" right="1" top="1.6666666666666701" bottom="1.6666666666666701" header="1" footer="1"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>

</xml_diff>

<commit_message>
New range for cryo test
</commit_message>
<xml_diff>
--- a/data/default_biases_cryo.xlsx
+++ b/data/default_biases_cryo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\zec\striptease\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\zec\Tesi\striptease\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F2EE7D-D14B-4B91-95E6-C1E84250819F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C92DA7-EBF7-477B-AAF3-8DFA3AC29390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,10 +881,10 @@
   <dimension ref="A1:BO41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AC18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AW23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD37" sqref="AD37"/>
+      <selection pane="bottomRight" activeCell="AC34" sqref="B34:AE37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7597,202 +7597,202 @@
         <v>99</v>
       </c>
       <c r="B34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="C34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="D34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="E34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="G34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="I34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="J34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L34" s="4">
-        <v>2170</v>
+        <v>2500</v>
       </c>
       <c r="M34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="N34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="O34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="P34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Q34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="R34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="S34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="T34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="U34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="V34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="W34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="X34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Y34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Z34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AA34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AB34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AC34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AD34" s="4">
-        <v>2150</v>
+        <v>2500</v>
       </c>
       <c r="AE34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AF34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AG34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AH34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AI34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AJ34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AK34" s="4">
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="AL34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AM34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AN34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AO34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AP34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AQ34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AR34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AS34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AT34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AU34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AV34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AW34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AX34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AY34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AZ34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BA34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BB34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BC34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BD34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BE34" s="4">
-        <v>2100</v>
+        <v>2500</v>
       </c>
       <c r="BF34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BG34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BH34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BI34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BJ34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BK34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BL34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BM34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BN34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BO34" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="35" spans="1:67">
@@ -7800,202 +7800,202 @@
         <v>100</v>
       </c>
       <c r="B35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="C35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="D35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="E35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="G35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="I35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="J35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L35" s="4">
-        <v>2170</v>
+        <v>2500</v>
       </c>
       <c r="M35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="N35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="O35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="P35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Q35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="R35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="S35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="T35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="U35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="V35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="W35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="X35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Y35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Z35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AA35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AB35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AC35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AD35" s="4">
-        <v>2150</v>
+        <v>2500</v>
       </c>
       <c r="AE35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AF35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AG35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AH35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AI35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AJ35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AK35" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="AL35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AM35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AN35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AO35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AP35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AQ35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AR35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AS35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AT35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AU35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AV35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AW35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AX35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AY35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AZ35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BA35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BB35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BC35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BD35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BE35" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="BF35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BG35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BH35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BI35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BJ35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BK35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BL35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BM35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BN35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BO35" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="36" spans="1:67">
@@ -8003,202 +8003,202 @@
         <v>101</v>
       </c>
       <c r="B36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="C36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="E36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="G36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="I36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="J36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L36" s="4">
-        <v>2150</v>
+        <v>2500</v>
       </c>
       <c r="M36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="N36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="O36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="P36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Q36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="R36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="S36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="T36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="U36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="V36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="W36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="X36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Y36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Z36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AA36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AB36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AC36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AD36" s="4">
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="AE36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AF36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AG36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AH36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AI36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AJ36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AK36" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="AL36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AM36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AN36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AO36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AP36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AQ36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AR36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AS36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AT36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AU36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AV36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AW36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AX36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AY36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AZ36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BA36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BB36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BC36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BD36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BE36" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="BF36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BG36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BH36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BI36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BJ36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BK36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BL36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BM36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BN36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BO36" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="37" spans="1:67">
@@ -8206,202 +8206,202 @@
         <v>102</v>
       </c>
       <c r="B37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="C37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="E37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="G37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="I37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="J37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="K37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="L37" s="4">
-        <v>2260</v>
+        <v>2500</v>
       </c>
       <c r="M37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="N37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="O37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="P37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Q37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="R37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="S37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="T37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="U37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="V37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="W37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="X37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Y37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="Z37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AA37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AB37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AC37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AD37" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="AE37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AF37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AG37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AH37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AI37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AJ37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AK37" s="4">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="AL37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AM37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AN37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AO37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AP37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AQ37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AR37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AS37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AT37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AU37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AV37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AW37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AX37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AY37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="AZ37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BA37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BB37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BC37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BD37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BE37" s="4">
-        <v>2150</v>
+        <v>2500</v>
       </c>
       <c r="BF37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BG37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BH37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BI37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BJ37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BK37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BL37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BM37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BN37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="BO37" s="4">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="38" spans="1:67">

</xml_diff>